<commit_message>
Changed BaselineTask command options
</commit_message>
<xml_diff>
--- a/Wattalyst.Sensors.xlsx
+++ b/Wattalyst.Sensors.xlsx
@@ -3224,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD157"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3663,23 +3663,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" s="2" customFormat="1">
+      <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>514</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>